<commit_message>
Přidány podklady pro kapacitní parametry plaveckých bazénů
</commit_message>
<xml_diff>
--- a/src/kapacita/kapacita.xlsx
+++ b/src/kapacita/kapacita.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="0" windowWidth="22395" windowHeight="14820"/>
+    <workbookView xWindow="6420" yWindow="0" windowWidth="22395" windowHeight="14820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>1 dráha</t>
-  </si>
-  <si>
-    <t>8 drah</t>
-  </si>
-  <si>
-    <t>10 drah</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>délka</t>
   </si>
@@ -47,12 +38,6 @@
     <t>m2/člověka *</t>
   </si>
   <si>
-    <t>dle hygienické normy / zákona</t>
-  </si>
-  <si>
-    <t>lidí max</t>
-  </si>
-  <si>
     <t>[m2]</t>
   </si>
   <si>
@@ -60,13 +45,49 @@
   </si>
   <si>
     <t>[-]</t>
+  </si>
+  <si>
+    <t>osob max</t>
+  </si>
+  <si>
+    <t>[osoby]</t>
+  </si>
+  <si>
+    <t>jedna dráha</t>
+  </si>
+  <si>
+    <t>dvě dráhy</t>
+  </si>
+  <si>
+    <t>polovina bazénu</t>
+  </si>
+  <si>
+    <t>celý bazén</t>
+  </si>
+  <si>
+    <t>Poznámka</t>
+  </si>
+  <si>
+    <t>drah</t>
+  </si>
+  <si>
+    <t>Nejvyšší přípustný počet osob v bazénu pro plavání dle  "bazénové" vyhlášky 238/2011 v platném znění</t>
+  </si>
+  <si>
+    <t>25m bazén - okamžitá kapacita - teoretická</t>
+  </si>
+  <si>
+    <t>25m bazén - okamžitá kapacita - praktická</t>
+  </si>
+  <si>
+    <t>Nejvyšší přijatelný počet osob v bazénu pro bezpečné plavání dle praktické zkušenosti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,16 +95,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -91,12 +147,164 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,122 +585,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <f>D4*C4</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="8">
+        <f>E4/B4</f>
+        <v>10</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>5</v>
+      </c>
+      <c r="C5" s="13">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14">
+        <f>D5*C5</f>
+        <v>100</v>
+      </c>
+      <c r="F5" s="15">
+        <f>E5/B5</f>
+        <v>20</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <f>D6*C6</f>
+        <v>300</v>
+      </c>
+      <c r="F6" s="8">
+        <f>E6/B6</f>
+        <v>60</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13">
+        <v>25</v>
+      </c>
+      <c r="D7" s="13">
+        <v>25</v>
+      </c>
+      <c r="E7" s="14">
+        <f>D7*C7</f>
+        <v>625</v>
+      </c>
+      <c r="F7" s="17">
+        <f>F4*10</f>
+        <v>100</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <f>D13*C13</f>
+        <v>50</v>
+      </c>
+      <c r="F13" s="8">
+        <f>E13/B13</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>2</v>
+      </c>
+      <c r="B14" s="18">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13">
+        <v>4</v>
+      </c>
+      <c r="E14" s="14">
+        <f>D14*C14</f>
+        <v>100</v>
+      </c>
+      <c r="F14" s="15">
+        <f>E14/B14</f>
+        <v>10</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4">
+        <v>25</v>
+      </c>
+      <c r="D15" s="4">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5">
+        <f>D15*C15</f>
+        <v>300</v>
+      </c>
+      <c r="F15" s="8">
+        <f>E15/B15</f>
+        <v>30</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
+        <v>6</v>
+      </c>
+      <c r="B16" s="18">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C16" s="13">
         <v>25</v>
       </c>
-      <c r="E3">
+      <c r="D16" s="13">
+        <v>25</v>
+      </c>
+      <c r="E16" s="14">
+        <f>D16*C16</f>
+        <v>625</v>
+      </c>
+      <c r="F16" s="17">
+        <f>F13*10</f>
         <v>50</v>
       </c>
-      <c r="F3">
-        <v>2.5</v>
-      </c>
-      <c r="G3">
-        <f>F3*E3</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f>G4/D4</f>
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <f>D3*8</f>
-        <v>200</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <f>F4*E4</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <f>G5/D5</f>
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <f>D3*10</f>
-        <v>250</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>25</v>
-      </c>
-      <c r="G5">
-        <f>F5*E5</f>
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>7</v>
+      <c r="G16" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
přidán seznam účastníků prezentace Myrtha Pools
</commit_message>
<xml_diff>
--- a/src/kapacita/kapacita.xlsx
+++ b/src/kapacita/kapacita.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="0" windowWidth="22395" windowHeight="14820"/>
+    <workbookView xWindow="7950" yWindow="0" windowWidth="22395" windowHeight="14820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>délka</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Nejvyšší přijatelný počet osob v bazénu pro bezpečné plavání dle praktické zkušenosti</t>
+  </si>
+  <si>
+    <t>25m bazén - okamžitá kapacita - praktická, šířka bazénu 12.5m (Městské lázně Prostějov)</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,6 +306,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -585,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,15 +732,15 @@
         <v>25</v>
       </c>
       <c r="D6" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5">
         <f>D6*C6</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="F6" s="8">
         <f>E6/B6</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>11</v>
@@ -733,11 +757,11 @@
         <v>25</v>
       </c>
       <c r="D7" s="13">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E7" s="14">
         <f>D7*C7</f>
-        <v>625</v>
+        <v>312.5</v>
       </c>
       <c r="F7" s="17">
         <f>F4*10</f>
@@ -862,15 +886,15 @@
         <v>25</v>
       </c>
       <c r="D15" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E15" s="5">
         <f>D15*C15</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="F15" s="8">
         <f>E15/B15</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>11</v>
@@ -887,11 +911,11 @@
         <v>25</v>
       </c>
       <c r="D16" s="13">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E16" s="14">
         <f>D16*C16</f>
-        <v>625</v>
+        <v>312.5</v>
       </c>
       <c r="F16" s="17">
         <f>F13*10</f>
@@ -901,9 +925,166 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>25</v>
+      </c>
+      <c r="D23" s="19">
+        <f>D26/6</f>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="E23" s="24">
+        <f>D23*C23</f>
+        <v>52.083333333333336</v>
+      </c>
+      <c r="F23" s="21">
+        <f>E23/B23</f>
+        <v>10.416666666666668</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>2</v>
+      </c>
+      <c r="B24" s="18">
+        <v>5</v>
+      </c>
+      <c r="C24" s="13">
+        <v>25</v>
+      </c>
+      <c r="D24" s="20">
+        <f>D26/3</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="E24" s="25">
+        <f>D24*C24</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="F24" s="22">
+        <f>E24/B24</f>
+        <v>20.833333333333336</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4">
+        <v>25</v>
+      </c>
+      <c r="D25" s="19">
+        <f>D26/2</f>
+        <v>6.25</v>
+      </c>
+      <c r="E25" s="24">
+        <f>D25*C25</f>
+        <v>156.25</v>
+      </c>
+      <c r="F25" s="21">
+        <f>E25/B25</f>
+        <v>31.25</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
+        <v>6</v>
+      </c>
+      <c r="B26" s="18">
+        <v>5</v>
+      </c>
+      <c r="C26" s="13">
+        <v>25</v>
+      </c>
+      <c r="D26" s="20">
+        <v>12.5</v>
+      </c>
+      <c r="E26" s="25">
+        <f>D26*C26</f>
+        <v>312.5</v>
+      </c>
+      <c r="F26" s="23">
+        <f>F23*10</f>
+        <v>104.16666666666669</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>